<commit_message>
jx: prefix, remove var prefix for groupBy, if:noElse testcase,
jxls-poi commands will be added automatically, withHideTemplateSheet()
removed, multisheet with objects testcase, useStreaming() for better
overriding and other small stuff
</commit_message>
<xml_diff>
--- a/jxls-poi/src/test/resources/org/jxls3/GridTest.xlsx
+++ b/jxls-poi/src/test/resources/org/jxls3/GridTest.xlsx
@@ -1,37 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{645774FF-98D9-4964-B00D-E3EE58AA54F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F57B09-6C8E-436F-93A7-0210B77D76A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26192" yWindow="-109" windowWidth="26301" windowHeight="14305"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -55,7 +44,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="0" shapeId="0">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -75,7 +64,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:grid(headers="headers" data="data" areas=[A3:A3, A4:A4] formatCells="BigDecimal:C1,Date:D1" lastCell="A4")</t>
+jx:grid(headers="headers" data="data" areas=["A3:A3","A4:A4"] formatCells="BigDecimal:C1,Date:D1" lastCell="A4")</t>
         </r>
       </text>
     </comment>
@@ -98,9 +87,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="[$-409]d/mmm/yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d/mmm/yy;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -179,7 +168,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -484,19 +473,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.625" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="32.950000000000003" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -506,12 +495,12 @@
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:6" ht="14.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>

</xml_diff>